<commit_message>
Final Changes after match 1
</commit_message>
<xml_diff>
--- a/CFC Fantasy League 2025.xlsx
+++ b/CFC Fantasy League 2025.xlsx
@@ -39,18 +39,18 @@
     <t>Tormented Titans</t>
   </si>
   <si>
+    <t>The Travelling Bankers</t>
+  </si>
+  <si>
     <t>Gujju Gang</t>
   </si>
   <si>
-    <t>The Travelling Bankers</t>
+    <t>Hilarious Hooligans</t>
   </si>
   <si>
     <t>Supa Jinx Strikas</t>
   </si>
   <si>
-    <t>Hilarious Hooligans</t>
-  </si>
-  <si>
     <t>Raging Raptors</t>
   </si>
   <si>
@@ -63,12 +63,18 @@
     <t>Krunal Pandya</t>
   </si>
   <si>
+    <t>Dhruv Jurel</t>
+  </si>
+  <si>
     <t>Travis Head</t>
   </si>
   <si>
     <t>Sunil Narine</t>
   </si>
   <si>
+    <t>Sanju Samson</t>
+  </si>
+  <si>
     <t>Ajinkya Rahane</t>
   </si>
   <si>
@@ -84,27 +90,30 @@
     <t>Tushar Deshpande</t>
   </si>
   <si>
-    <t>Sanju Samson</t>
+    <t>Harshal Patel</t>
   </si>
   <si>
     <t>Abhishek Sharma</t>
   </si>
   <si>
+    <t>Shimron Hetmyer</t>
+  </si>
+  <si>
+    <t>Heinrich Klaasen</t>
+  </si>
+  <si>
+    <t>Shubham Dubey</t>
+  </si>
+  <si>
+    <t>Rajat Patidar</t>
+  </si>
+  <si>
+    <t>Liam Livingstone</t>
+  </si>
+  <si>
     <t>Simarjeet Singh</t>
   </si>
   <si>
-    <t>Dhruv Jurel</t>
-  </si>
-  <si>
-    <t>Heinrich Klaasen</t>
-  </si>
-  <si>
-    <t>Rajat Patidar</t>
-  </si>
-  <si>
-    <t>Liam Livingstone</t>
-  </si>
-  <si>
     <t>Maheesh Theekshana</t>
   </si>
   <si>
@@ -135,6 +144,9 @@
     <t>Mohammed Shami</t>
   </si>
   <si>
+    <t>Adam Zampa</t>
+  </si>
+  <si>
     <t>Devdutt Padikkal</t>
   </si>
   <si>
@@ -147,21 +159,21 @@
     <t>Yashasvi Jaiswal</t>
   </si>
   <si>
+    <t>Harshit Rana</t>
+  </si>
+  <si>
+    <t>Vaibhav Arora</t>
+  </si>
+  <si>
+    <t>Aniket Verma</t>
+  </si>
+  <si>
+    <t>Abhinav Manohar</t>
+  </si>
+  <si>
     <t>Pat Cummins</t>
   </si>
   <si>
-    <t>Harshit Rana</t>
-  </si>
-  <si>
-    <t>Vaibhav Arora</t>
-  </si>
-  <si>
-    <t>Aniket Verma</t>
-  </si>
-  <si>
-    <t>Shimron Hetmyer</t>
-  </si>
-  <si>
     <t>Venkatesh Iyer</t>
   </si>
   <si>
@@ -174,19 +186,7 @@
     <t>Spencer Johnson</t>
   </si>
   <si>
-    <t>Harshal Patel</t>
-  </si>
-  <si>
-    <t>Adam Zampa</t>
-  </si>
-  <si>
     <t>Nitish Kumar Reddy</t>
-  </si>
-  <si>
-    <t>Abhinav Manohar</t>
-  </si>
-  <si>
-    <t>Shubham Dubey</t>
   </si>
   <si>
     <t>Tim David</t>
@@ -1121,7 +1121,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>586</v>
+        <v>643</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>225</v>
+        <v>282</v>
       </c>
       <c r="F2">
         <v>361</v>
@@ -1141,7 +1141,7 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>520.5</v>
+        <v>640</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1150,10 +1150,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>280.5</v>
+        <v>187</v>
       </c>
       <c r="F3">
-        <v>240</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1161,7 +1161,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>455</v>
+        <v>520.5</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1170,10 +1170,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>280.5</v>
       </c>
       <c r="F4">
-        <v>453</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1181,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>400</v>
+        <v>471</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1190,10 +1190,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>264</v>
+        <v>356</v>
       </c>
       <c r="F5">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1201,7 +1201,7 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>365</v>
+        <v>441</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1210,10 +1210,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>250</v>
+        <v>305</v>
       </c>
       <c r="F6">
-        <v>115</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1221,7 +1221,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F7">
         <v>236</v>
@@ -1241,7 +1241,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="F8">
         <v>222</v>
@@ -1291,7 +1291,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1300,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1360,10 +1360,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="F5">
-        <v>148</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1371,7 +1371,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1391,7 +1391,7 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1400,10 +1400,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="F7">
-        <v>135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1411,7 +1411,7 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1431,7 +1431,7 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1443,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1451,7 +1451,7 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1460,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1471,7 +1471,7 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1480,10 +1480,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1491,7 +1491,7 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1511,7 +1511,7 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1520,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1531,7 +1531,7 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1551,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1571,7 +1571,7 @@
         <v>26</v>
       </c>
       <c r="B16">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1580,10 +1580,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="F16">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1591,7 +1591,7 @@
         <v>27</v>
       </c>
       <c r="B17">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1600,10 +1600,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F17">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1611,7 +1611,7 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1620,10 +1620,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1631,7 +1631,7 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1651,7 +1651,7 @@
         <v>30</v>
       </c>
       <c r="B20">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1660,10 +1660,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="F20">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1671,7 +1671,7 @@
         <v>31</v>
       </c>
       <c r="B21">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1680,10 +1680,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="F21">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1691,7 +1691,7 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1711,7 +1711,7 @@
         <v>33</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1723,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1731,7 +1731,7 @@
         <v>34</v>
       </c>
       <c r="B24">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1743,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1751,7 +1751,7 @@
         <v>35</v>
       </c>
       <c r="B25">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1771,7 +1771,7 @@
         <v>36</v>
       </c>
       <c r="B26">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1780,10 +1780,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1791,7 +1791,7 @@
         <v>37</v>
       </c>
       <c r="B27">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1800,10 +1800,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1811,7 +1811,7 @@
         <v>38</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1823,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1831,7 +1831,7 @@
         <v>39</v>
       </c>
       <c r="B29">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1851,7 +1851,7 @@
         <v>40</v>
       </c>
       <c r="B30">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1871,7 +1871,7 @@
         <v>41</v>
       </c>
       <c r="B31">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1891,7 +1891,7 @@
         <v>42</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1900,10 +1900,10 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1911,7 +1911,7 @@
         <v>43</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1920,10 +1920,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F33">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1931,7 +1931,7 @@
         <v>44</v>
       </c>
       <c r="B34">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1940,10 +1940,10 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F34">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1951,7 +1951,7 @@
         <v>45</v>
       </c>
       <c r="B35">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1971,7 +1971,7 @@
         <v>46</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1980,10 +1980,10 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1991,7 +1991,7 @@
         <v>47</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2003,7 +2003,7 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2011,7 +2011,7 @@
         <v>48</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2020,10 +2020,10 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F38">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2031,7 +2031,7 @@
         <v>49</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2040,10 +2040,10 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F39">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2051,7 +2051,7 @@
         <v>50</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2060,10 +2060,10 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2071,7 +2071,7 @@
         <v>51</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2080,10 +2080,10 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2091,7 +2091,7 @@
         <v>52</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2100,10 +2100,10 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2111,7 +2111,7 @@
         <v>53</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2123,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2131,7 +2131,7 @@
         <v>54</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2211,7 +2211,7 @@
         <v>58</v>
       </c>
       <c r="B48">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>149</v>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>96</v>
@@ -2609,10 +2609,10 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>99</v>
@@ -2693,13 +2693,13 @@
         <v>0</v>
       </c>
       <c r="AD4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG4">
         <v>0</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2838,10 +2838,10 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2925,13 +2925,13 @@
         <v>0</v>
       </c>
       <c r="AD6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG6">
         <v>0</v>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -3067,10 +3067,10 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3154,13 +3154,13 @@
         <v>0</v>
       </c>
       <c r="AD8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AG8">
         <v>0</v>
@@ -3183,10 +3183,10 @@
     </row>
     <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3228,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -3243,16 +3243,16 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -3299,10 +3299,10 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B10">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -3356,16 +3356,16 @@
         <v>50</v>
       </c>
       <c r="U10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V10">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="W10">
-        <v>10</v>
+        <v>15.33</v>
       </c>
       <c r="X10">
-        <v>5</v>
+        <v>-20</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -3412,10 +3412,10 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3457,31 +3457,31 @@
         <v>0</v>
       </c>
       <c r="P11">
+        <v>109</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
         <v>2</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
       <c r="T11">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="U11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="V11">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="W11">
-        <v>3</v>
+        <v>8.5</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Y11">
         <v>0</v>
@@ -3496,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AD11">
         <v>0</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>31</v>
@@ -3644,10 +3644,10 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -3689,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -3698,22 +3698,22 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="V13">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="W13">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="Y13">
         <v>0</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>21</v>
@@ -3876,10 +3876,10 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -3888,31 +3888,31 @@
         <v>97</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>309.09</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>35</v>
@@ -4108,7 +4108,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>26</v>
@@ -4224,10 +4224,10 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -4236,13 +4236,13 @@
         <v>99</v>
       </c>
       <c r="E18">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="F18">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="G18">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="H18">
         <v>5</v>
@@ -4251,13 +4251,13 @@
         <v>10</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K18">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="L18">
-        <v>237.5</v>
+        <v>200</v>
       </c>
       <c r="M18">
         <v>30</v>
@@ -4266,7 +4266,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -4340,10 +4340,10 @@
     </row>
     <row r="19" spans="1:38">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -4352,31 +4352,31 @@
         <v>97</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>182.6</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -4459,7 +4459,7 @@
         <v>58</v>
       </c>
       <c r="B20">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -4468,13 +4468,13 @@
         <v>100</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -4489,7 +4489,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="21" spans="1:38">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>71</v>
@@ -4688,7 +4688,7 @@
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>121</v>
@@ -4804,7 +4804,7 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B23">
         <v>25</v>
@@ -5033,10 +5033,10 @@
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -5045,28 +5045,28 @@
         <v>99</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F25">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G25">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="H25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I25">
+        <v>14</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
         <v>12</v>
       </c>
-      <c r="J25">
-        <v>3</v>
-      </c>
-      <c r="K25">
-        <v>9</v>
-      </c>
       <c r="L25">
-        <v>196</v>
+        <v>178.37</v>
       </c>
       <c r="M25">
         <v>30</v>
@@ -5075,7 +5075,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="P25">
         <v>0</v>
@@ -5168,13 +5168,13 @@
         <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>102</v>
@@ -5195,7 +5195,7 @@
         <v>107</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>108</v>
@@ -5210,7 +5210,7 @@
         <v>111</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>112</v>
@@ -5219,7 +5219,7 @@
         <v>113</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>114</v>
@@ -5252,7 +5252,7 @@
         <v>123</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>124</v>
@@ -5261,10 +5261,10 @@
         <v>125</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>126</v>
@@ -5285,7 +5285,7 @@
         <v>131</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>132</v>
@@ -5297,13 +5297,13 @@
         <v>134</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>136</v>
@@ -5324,7 +5324,7 @@
         <v>141</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>142</v>
@@ -5336,16 +5336,16 @@
         <v>144</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="BI1" s="1" t="s">
         <v>145</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>146</v>
@@ -5357,13 +5357,13 @@
         <v>148</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>150</v>
@@ -5393,16 +5393,16 @@
         <v>157</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>158</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>159</v>
@@ -5426,10 +5426,10 @@
         <v>165</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="CN1" s="1" t="s">
         <v>166</v>
@@ -5456,7 +5456,7 @@
         <v>173</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>174</v>
@@ -5468,10 +5468,10 @@
         <v>176</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>177</v>
@@ -5486,7 +5486,7 @@
         <v>180</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>181</v>
@@ -5516,7 +5516,7 @@
         <v>188</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>189</v>
@@ -5525,7 +5525,7 @@
         <v>190</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="DT1" s="1" t="s">
         <v>191</v>
@@ -5567,7 +5567,7 @@
         <v>201</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>202</v>
@@ -5597,7 +5597,7 @@
         <v>210</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>211</v>
@@ -5615,7 +5615,7 @@
         <v>214</v>
       </c>
       <c r="EW1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="EX1" s="1" t="s">
         <v>215</v>
@@ -5633,13 +5633,13 @@
         <v>219</v>
       </c>
       <c r="FC1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>220</v>
@@ -5651,7 +5651,7 @@
         <v>222</v>
       </c>
       <c r="FI1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="FJ1" s="1" t="s">
         <v>223</v>
@@ -5663,7 +5663,7 @@
         <v>225</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>226</v>
@@ -5681,7 +5681,7 @@
         <v>230</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>231</v>
@@ -5707,7 +5707,7 @@
     </row>
     <row r="2" spans="1:182">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>280.5</v>
@@ -6255,10 +6255,10 @@
     </row>
     <row r="3" spans="1:182">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>356</v>
       </c>
       <c r="C3" t="s">
         <v>238</v>
@@ -6357,7 +6357,7 @@
         <v>0</v>
       </c>
       <c r="AI3">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="AJ3">
         <v>0</v>
@@ -6393,13 +6393,13 @@
         <v>0</v>
       </c>
       <c r="AU3">
+        <v>96</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
         <v>10</v>
-      </c>
-      <c r="AV3">
-        <v>0</v>
-      </c>
-      <c r="AW3">
-        <v>0</v>
       </c>
       <c r="AX3">
         <v>0</v>
@@ -6806,7 +6806,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>225</v>
+        <v>282</v>
       </c>
       <c r="C4" t="s">
         <v>238</v>
@@ -7007,7 +7007,7 @@
         <v>0</v>
       </c>
       <c r="BQ4">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="BR4">
         <v>0</v>
@@ -7043,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="CC4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="CD4">
         <v>0</v>
@@ -7354,7 +7354,7 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
         <v>238</v>
@@ -7660,7 +7660,7 @@
         <v>0</v>
       </c>
       <c r="CZ5">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="DA5">
         <v>0</v>
@@ -7899,10 +7899,10 @@
     </row>
     <row r="6" spans="1:182">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>264</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s">
         <v>238</v>
@@ -8247,7 +8247,7 @@
         <v>0</v>
       </c>
       <c r="DM6">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="DN6">
         <v>0</v>
@@ -8292,7 +8292,7 @@
         <v>0</v>
       </c>
       <c r="EB6">
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="EC6">
         <v>0</v>
@@ -8450,7 +8450,7 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>238</v>
@@ -8903,7 +8903,7 @@
         <v>0</v>
       </c>
       <c r="EW7">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="EX7">
         <v>0</v>
@@ -8995,10 +8995,10 @@
     </row>
     <row r="8" spans="1:182">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s">
         <v>238</v>
@@ -9475,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="FE8">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="FF8">
         <v>0</v>
@@ -9499,7 +9499,7 @@
         <v>0</v>
       </c>
       <c r="FM8">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="FN8">
         <v>0</v>
@@ -9669,7 +9669,7 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -9785,7 +9785,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -9901,7 +9901,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>135</v>
@@ -10017,7 +10017,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>39</v>
@@ -10133,7 +10133,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>57</v>
@@ -10249,7 +10249,7 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>148</v>
@@ -10365,7 +10365,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -10597,7 +10597,7 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -10713,7 +10713,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -10829,7 +10829,7 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>44</v>
@@ -10945,7 +10945,7 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>13</v>
@@ -11061,7 +11061,7 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>131</v>
@@ -11177,7 +11177,7 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>135</v>
@@ -11293,7 +11293,7 @@
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>77</v>
@@ -11409,7 +11409,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>76</v>
@@ -11525,7 +11525,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -11873,7 +11873,7 @@
     </row>
     <row r="21" spans="1:38">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>43</v>
@@ -11989,7 +11989,7 @@
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>39</v>
@@ -12105,7 +12105,7 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>132</v>
@@ -12221,7 +12221,7 @@
     </row>
     <row r="24" spans="1:38">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>59</v>
@@ -12337,7 +12337,7 @@
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B25">
         <v>27</v>
@@ -12472,13 +12472,13 @@
         <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>102</v>
@@ -12499,7 +12499,7 @@
         <v>107</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>108</v>
@@ -12514,7 +12514,7 @@
         <v>111</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>112</v>
@@ -12523,7 +12523,7 @@
         <v>113</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>114</v>
@@ -12556,7 +12556,7 @@
         <v>123</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>124</v>
@@ -12565,10 +12565,10 @@
         <v>125</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>126</v>
@@ -12589,7 +12589,7 @@
         <v>131</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>132</v>
@@ -12601,13 +12601,13 @@
         <v>134</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>135</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>136</v>
@@ -12628,7 +12628,7 @@
         <v>141</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>142</v>
@@ -12640,16 +12640,16 @@
         <v>144</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="BI1" s="1" t="s">
         <v>145</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>146</v>
@@ -12661,13 +12661,13 @@
         <v>148</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>150</v>
@@ -12697,16 +12697,16 @@
         <v>157</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>158</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>159</v>
@@ -12730,10 +12730,10 @@
         <v>165</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="CN1" s="1" t="s">
         <v>166</v>
@@ -12748,7 +12748,7 @@
         <v>169</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>171</v>
@@ -12760,7 +12760,7 @@
         <v>173</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>174</v>
@@ -12772,10 +12772,10 @@
         <v>176</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>177</v>
@@ -12790,7 +12790,7 @@
         <v>180</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>181</v>
@@ -12820,7 +12820,7 @@
         <v>188</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>189</v>
@@ -12829,7 +12829,7 @@
         <v>190</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="DT1" s="1" t="s">
         <v>191</v>
@@ -12871,7 +12871,7 @@
         <v>201</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>202</v>
@@ -12901,7 +12901,7 @@
         <v>210</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>211</v>
@@ -12919,7 +12919,7 @@
         <v>214</v>
       </c>
       <c r="EW1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="EX1" s="1" t="s">
         <v>215</v>
@@ -12937,13 +12937,13 @@
         <v>219</v>
       </c>
       <c r="FC1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>220</v>
@@ -12955,7 +12955,7 @@
         <v>222</v>
       </c>
       <c r="FI1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="FJ1" s="1" t="s">
         <v>223</v>
@@ -12967,7 +12967,7 @@
         <v>225</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>226</v>
@@ -12985,7 +12985,7 @@
         <v>230</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>231</v>
@@ -13011,7 +13011,7 @@
     </row>
     <row r="2" spans="1:182">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>240</v>
@@ -13559,7 +13559,7 @@
     </row>
     <row r="3" spans="1:182">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>115</v>
@@ -15203,7 +15203,7 @@
     </row>
     <row r="6" spans="1:182">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>136</v>
@@ -16299,7 +16299,7 @@
     </row>
     <row r="8" spans="1:182">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>453</v>

</xml_diff>

<commit_message>
its philip salt not phil salt
</commit_message>
<xml_diff>
--- a/CFC Fantasy League 2025.xlsx
+++ b/CFC Fantasy League 2025.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="237">
   <si>
     <t>Total Points</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Ajinkya Rahane</t>
+  </si>
+  <si>
+    <t>Philip Salt</t>
   </si>
   <si>
     <t>Josh Hazlewood</t>
@@ -293,9 +296,6 @@
   </si>
   <si>
     <t>Jake Fraser-McGurk</t>
-  </si>
-  <si>
-    <t>Phil Salt</t>
   </si>
   <si>
     <t>Tim David</t>
@@ -735,9 +735,6 @@
   <si>
     <t>None</t>
   </si>
-  <si>
-    <t>Philip Salt</t>
-  </si>
 </sst>
 </file>
 
@@ -1326,13 +1323,13 @@
         <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>142</v>
@@ -1347,13 +1344,13 @@
         <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>19</v>
@@ -1362,28 +1359,28 @@
         <v>147</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>148</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>150</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>151</v>
@@ -1410,19 +1407,19 @@
         <v>158</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>160</v>
@@ -1440,13 +1437,13 @@
         <v>164</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>165</v>
@@ -1455,19 +1452,19 @@
         <v>166</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>167</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>168</v>
@@ -1482,7 +1479,7 @@
         <v>171</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>14</v>
@@ -1494,16 +1491,16 @@
         <v>173</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>174</v>
@@ -1515,7 +1512,7 @@
         <v>95</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>27</v>
@@ -1524,7 +1521,7 @@
         <v>22</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>176</v>
@@ -1551,19 +1548,19 @@
         <v>182</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>183</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="CF1" s="1" t="s">
         <v>184</v>
@@ -1584,16 +1581,16 @@
         <v>189</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CP1" s="1" t="s">
         <v>191</v>
@@ -1602,10 +1599,10 @@
         <v>192</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>237</v>
+        <v>29</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CT1" s="1" t="s">
         <v>93</v>
@@ -1614,22 +1611,22 @@
         <v>193</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>194</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>195</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>196</v>
@@ -1644,7 +1641,7 @@
         <v>199</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>200</v>
@@ -1653,10 +1650,10 @@
         <v>26</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="DK1" s="1" t="s">
         <v>201</v>
@@ -1674,19 +1671,19 @@
         <v>203</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>204</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="DT1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="DU1" s="1" t="s">
         <v>205</v>
@@ -1698,7 +1695,7 @@
         <v>91</v>
       </c>
       <c r="DX1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="DY1" s="1" t="s">
         <v>207</v>
@@ -1707,7 +1704,7 @@
         <v>208</v>
       </c>
       <c r="EA1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="EB1" s="1" t="s">
         <v>96</v>
@@ -1725,16 +1722,16 @@
         <v>212</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>213</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="EK1" s="1" t="s">
         <v>214</v>
@@ -1743,7 +1740,7 @@
         <v>215</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="EN1" s="1" t="s">
         <v>216</v>
@@ -1755,13 +1752,13 @@
         <v>218</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>99</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="ET1" s="1" t="s">
         <v>219</v>
@@ -1794,10 +1791,10 @@
         <v>24</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>225</v>
@@ -1815,22 +1812,22 @@
         <v>228</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="FL1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>230</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="FQ1" s="1" t="s">
         <v>231</v>
@@ -1839,13 +1836,13 @@
         <v>232</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="FV1" s="1" t="s">
         <v>98</v>
@@ -6130,7 +6127,7 @@
         <v>29</v>
       </c>
       <c r="B17">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -6145,7 +6142,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -6156,7 +6153,7 @@
         <v>30</v>
       </c>
       <c r="B18">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -6171,7 +6168,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -6182,7 +6179,7 @@
         <v>31</v>
       </c>
       <c r="B19">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -6191,13 +6188,13 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -6208,7 +6205,7 @@
         <v>32</v>
       </c>
       <c r="B20">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -6217,10 +6214,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="F20">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -6234,7 +6231,7 @@
         <v>33</v>
       </c>
       <c r="B21">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -6243,10 +6240,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -6260,7 +6257,7 @@
         <v>34</v>
       </c>
       <c r="B22">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -6269,10 +6266,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="F22">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -6286,7 +6283,7 @@
         <v>35</v>
       </c>
       <c r="B23">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -6298,13 +6295,13 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -6312,7 +6309,7 @@
         <v>36</v>
       </c>
       <c r="B24">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -6330,7 +6327,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -6338,7 +6335,7 @@
         <v>37</v>
       </c>
       <c r="B25">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -6350,13 +6347,13 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -6390,7 +6387,7 @@
         <v>39</v>
       </c>
       <c r="B27">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -6399,10 +6396,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -6416,7 +6413,7 @@
         <v>40</v>
       </c>
       <c r="B28">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -6425,7 +6422,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -6442,7 +6439,7 @@
         <v>41</v>
       </c>
       <c r="B29">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -6451,10 +6448,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F29">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -6468,7 +6465,7 @@
         <v>42</v>
       </c>
       <c r="B30">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -6480,13 +6477,13 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -6494,7 +6491,7 @@
         <v>43</v>
       </c>
       <c r="B31">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -6506,13 +6503,13 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -6520,7 +6517,7 @@
         <v>44</v>
       </c>
       <c r="B32">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -6532,10 +6529,10 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="G32">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -6546,7 +6543,7 @@
         <v>45</v>
       </c>
       <c r="B33">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -6561,7 +6558,7 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -6572,7 +6569,7 @@
         <v>46</v>
       </c>
       <c r="B34">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -6587,10 +6584,10 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="H34">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -6610,13 +6607,13 @@
         <v>0</v>
       </c>
       <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>71</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -6650,7 +6647,7 @@
         <v>49</v>
       </c>
       <c r="B37">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -6659,10 +6656,10 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -6676,7 +6673,7 @@
         <v>50</v>
       </c>
       <c r="B38">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -6685,7 +6682,7 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -6694,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -6711,16 +6708,16 @@
         <v>0</v>
       </c>
       <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
         <v>65</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -6728,7 +6725,7 @@
         <v>52</v>
       </c>
       <c r="B40">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -6737,13 +6734,13 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -6754,7 +6751,7 @@
         <v>53</v>
       </c>
       <c r="B41">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -6763,13 +6760,13 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -6789,13 +6786,13 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -6806,7 +6803,7 @@
         <v>55</v>
       </c>
       <c r="B43">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -6815,13 +6812,13 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -6832,7 +6829,7 @@
         <v>56</v>
       </c>
       <c r="B44">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -6841,7 +6838,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -6858,7 +6855,7 @@
         <v>57</v>
       </c>
       <c r="B45">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -6867,13 +6864,13 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -6884,7 +6881,7 @@
         <v>58</v>
       </c>
       <c r="B46">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -6899,7 +6896,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -6910,7 +6907,7 @@
         <v>59</v>
       </c>
       <c r="B47">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -6925,7 +6922,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -6962,7 +6959,7 @@
         <v>61</v>
       </c>
       <c r="B49">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -6977,10 +6974,10 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H49">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -7000,13 +6997,13 @@
         <v>0</v>
       </c>
       <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
         <v>35</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -7014,7 +7011,7 @@
         <v>63</v>
       </c>
       <c r="B51">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -7023,10 +7020,10 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -7040,7 +7037,7 @@
         <v>64</v>
       </c>
       <c r="B52">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -7049,7 +7046,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -7066,7 +7063,7 @@
         <v>65</v>
       </c>
       <c r="B53">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -7075,10 +7072,10 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F53">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -7092,7 +7089,7 @@
         <v>66</v>
       </c>
       <c r="B54">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -7104,7 +7101,7 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -7118,7 +7115,7 @@
         <v>67</v>
       </c>
       <c r="B55">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -7130,13 +7127,13 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
       <c r="H55">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -7144,7 +7141,7 @@
         <v>68</v>
       </c>
       <c r="B56">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -7159,10 +7156,10 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -7170,7 +7167,7 @@
         <v>69</v>
       </c>
       <c r="B57">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -7182,10 +7179,10 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -7196,7 +7193,7 @@
         <v>70</v>
       </c>
       <c r="B58">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -7208,7 +7205,7 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -7222,7 +7219,7 @@
         <v>71</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -7234,13 +7231,13 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G59">
         <v>0</v>
       </c>
       <c r="H59">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -7248,7 +7245,7 @@
         <v>72</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -7260,13 +7257,13 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G60">
         <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -7274,7 +7271,7 @@
         <v>73</v>
       </c>
       <c r="B61">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -7286,13 +7283,13 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G61">
         <v>0</v>
       </c>
       <c r="H61">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -7341,10 +7338,10 @@
         <v>0</v>
       </c>
       <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
         <v>20</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -7352,7 +7349,7 @@
         <v>76</v>
       </c>
       <c r="B64">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -7367,10 +7364,10 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H64">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -7387,16 +7384,16 @@
         <v>0</v>
       </c>
       <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
         <v>14</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -7404,7 +7401,7 @@
         <v>78</v>
       </c>
       <c r="B66">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -7413,13 +7410,13 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F66">
         <v>0</v>
       </c>
       <c r="G66">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -7430,7 +7427,7 @@
         <v>79</v>
       </c>
       <c r="B67">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -7439,13 +7436,13 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F67">
         <v>0</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -7465,10 +7462,10 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F68">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -7482,7 +7479,7 @@
         <v>81</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -7494,7 +7491,7 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -7520,10 +7517,10 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G70">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -7534,7 +7531,7 @@
         <v>83</v>
       </c>
       <c r="B71">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -7549,10 +7546,10 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H71">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -7575,10 +7572,10 @@
         <v>0</v>
       </c>
       <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
         <v>6</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -7612,7 +7609,7 @@
         <v>86</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -7627,7 +7624,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -7638,7 +7635,7 @@
         <v>87</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -7647,13 +7644,13 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F75">
         <v>0</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -7664,7 +7661,7 @@
         <v>88</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -7673,7 +7670,7 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -7690,7 +7687,7 @@
         <v>89</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -7699,7 +7696,7 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -7708,7 +7705,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -7716,7 +7713,7 @@
         <v>90</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -7734,7 +7731,7 @@
         <v>0</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -8099,7 +8096,7 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8215,7 +8212,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>81</v>
@@ -8447,7 +8444,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -8563,7 +8560,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>105</v>
@@ -8679,7 +8676,7 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>97</v>
@@ -9027,7 +9024,7 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -9143,7 +9140,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>23</v>
@@ -9375,7 +9372,7 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>35</v>
@@ -9723,7 +9720,7 @@
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -9839,7 +9836,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B17">
         <v>20</v>
@@ -9955,7 +9952,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18">
         <v>65</v>
@@ -10071,7 +10068,7 @@
     </row>
     <row r="19" spans="1:38">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19">
         <v>28</v>
@@ -10187,7 +10184,7 @@
     </row>
     <row r="20" spans="1:38">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>71</v>
@@ -10322,13 +10319,13 @@
         <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>142</v>
@@ -10343,13 +10340,13 @@
         <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>19</v>
@@ -10358,28 +10355,28 @@
         <v>147</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>148</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>150</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>151</v>
@@ -10406,19 +10403,19 @@
         <v>158</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>160</v>
@@ -10436,13 +10433,13 @@
         <v>164</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>165</v>
@@ -10451,19 +10448,19 @@
         <v>166</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>167</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>168</v>
@@ -10478,7 +10475,7 @@
         <v>171</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>14</v>
@@ -10490,16 +10487,16 @@
         <v>173</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>174</v>
@@ -10511,7 +10508,7 @@
         <v>95</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>27</v>
@@ -10520,7 +10517,7 @@
         <v>22</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>176</v>
@@ -10547,19 +10544,19 @@
         <v>182</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>183</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="CF1" s="1" t="s">
         <v>184</v>
@@ -10580,16 +10577,16 @@
         <v>189</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CP1" s="1" t="s">
         <v>191</v>
@@ -10598,10 +10595,10 @@
         <v>192</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CT1" s="1" t="s">
         <v>93</v>
@@ -10610,22 +10607,22 @@
         <v>193</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>194</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>195</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>196</v>
@@ -10640,7 +10637,7 @@
         <v>199</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>200</v>
@@ -10649,10 +10646,10 @@
         <v>26</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="DK1" s="1" t="s">
         <v>201</v>
@@ -10670,19 +10667,19 @@
         <v>203</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>204</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="DT1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="DU1" s="1" t="s">
         <v>205</v>
@@ -10694,7 +10691,7 @@
         <v>91</v>
       </c>
       <c r="DX1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="DY1" s="1" t="s">
         <v>207</v>
@@ -10703,7 +10700,7 @@
         <v>208</v>
       </c>
       <c r="EA1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="EB1" s="1" t="s">
         <v>96</v>
@@ -10721,16 +10718,16 @@
         <v>212</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>213</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="EK1" s="1" t="s">
         <v>214</v>
@@ -10739,7 +10736,7 @@
         <v>215</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="EN1" s="1" t="s">
         <v>216</v>
@@ -10751,13 +10748,13 @@
         <v>218</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>99</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="ET1" s="1" t="s">
         <v>219</v>
@@ -10790,10 +10787,10 @@
         <v>24</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>225</v>
@@ -10811,22 +10808,22 @@
         <v>228</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="FL1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>230</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="FQ1" s="1" t="s">
         <v>231</v>
@@ -10835,13 +10832,13 @@
         <v>232</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="FV1" s="1" t="s">
         <v>98</v>
@@ -14939,7 +14936,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>126</v>
@@ -15055,7 +15052,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -15171,7 +15168,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -15287,7 +15284,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>65</v>
@@ -15519,7 +15516,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -15635,7 +15632,7 @@
     </row>
     <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>57</v>
@@ -15867,7 +15864,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -16099,7 +16096,7 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -16331,7 +16328,7 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>34</v>
@@ -16447,7 +16444,7 @@
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>92</v>
@@ -16563,7 +16560,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>51</v>
@@ -16679,7 +16676,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>66</v>
@@ -16795,7 +16792,7 @@
     </row>
     <row r="19" spans="1:38">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19">
         <v>88</v>
@@ -17143,7 +17140,7 @@
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>118</v>
@@ -17259,7 +17256,7 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>14</v>
@@ -17394,13 +17391,13 @@
         <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>142</v>
@@ -17415,13 +17412,13 @@
         <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>19</v>
@@ -17430,28 +17427,28 @@
         <v>147</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>148</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>150</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>151</v>
@@ -17478,19 +17475,19 @@
         <v>158</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>160</v>
@@ -17508,13 +17505,13 @@
         <v>164</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>165</v>
@@ -17523,19 +17520,19 @@
         <v>166</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>167</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>168</v>
@@ -17550,7 +17547,7 @@
         <v>171</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>14</v>
@@ -17562,16 +17559,16 @@
         <v>173</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>174</v>
@@ -17583,7 +17580,7 @@
         <v>95</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>27</v>
@@ -17592,7 +17589,7 @@
         <v>22</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>176</v>
@@ -17619,19 +17616,19 @@
         <v>182</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>183</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="CF1" s="1" t="s">
         <v>184</v>
@@ -17652,16 +17649,16 @@
         <v>189</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CP1" s="1" t="s">
         <v>191</v>
@@ -17670,10 +17667,10 @@
         <v>192</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CT1" s="1" t="s">
         <v>93</v>
@@ -17682,22 +17679,22 @@
         <v>193</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>194</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>195</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>196</v>
@@ -17712,7 +17709,7 @@
         <v>199</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>200</v>
@@ -17721,10 +17718,10 @@
         <v>26</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="DK1" s="1" t="s">
         <v>201</v>
@@ -17742,19 +17739,19 @@
         <v>203</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>204</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="DT1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="DU1" s="1" t="s">
         <v>205</v>
@@ -17766,7 +17763,7 @@
         <v>91</v>
       </c>
       <c r="DX1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="DY1" s="1" t="s">
         <v>207</v>
@@ -17775,7 +17772,7 @@
         <v>208</v>
       </c>
       <c r="EA1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="EB1" s="1" t="s">
         <v>96</v>
@@ -17793,16 +17790,16 @@
         <v>212</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>213</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="EK1" s="1" t="s">
         <v>214</v>
@@ -17811,7 +17808,7 @@
         <v>215</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="EN1" s="1" t="s">
         <v>216</v>
@@ -17823,13 +17820,13 @@
         <v>218</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>99</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="ET1" s="1" t="s">
         <v>219</v>
@@ -17862,10 +17859,10 @@
         <v>24</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>225</v>
@@ -17883,22 +17880,22 @@
         <v>228</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="FL1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>230</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="FQ1" s="1" t="s">
         <v>231</v>
@@ -17907,13 +17904,13 @@
         <v>232</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="FV1" s="1" t="s">
         <v>98</v>
@@ -22011,7 +22008,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>96</v>
@@ -22243,7 +22240,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>71</v>
@@ -22359,7 +22356,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>87</v>
@@ -22475,7 +22472,7 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -22591,7 +22588,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -22707,7 +22704,7 @@
     </row>
     <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>109</v>
@@ -22823,7 +22820,7 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>31</v>
@@ -22939,7 +22936,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>29</v>
@@ -23055,7 +23052,7 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B12">
         <v>21</v>
@@ -23171,7 +23168,7 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13">
         <v>78</v>
@@ -23287,7 +23284,7 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -23403,7 +23400,7 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B15">
         <v>26</v>
@@ -23635,7 +23632,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>96</v>
@@ -23867,7 +23864,7 @@
     </row>
     <row r="19" spans="1:38">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>71</v>
@@ -23983,7 +23980,7 @@
     </row>
     <row r="20" spans="1:38">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>121</v>
@@ -24099,7 +24096,7 @@
     </row>
     <row r="21" spans="1:38">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>25</v>
@@ -24350,13 +24347,13 @@
         <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>142</v>
@@ -24371,13 +24368,13 @@
         <v>145</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>146</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>19</v>
@@ -24386,28 +24383,28 @@
         <v>147</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>148</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>149</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>150</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>151</v>
@@ -24434,19 +24431,19 @@
         <v>158</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>159</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>160</v>
@@ -24464,13 +24461,13 @@
         <v>164</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>165</v>
@@ -24479,19 +24476,19 @@
         <v>166</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>167</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AX1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>168</v>
@@ -24506,7 +24503,7 @@
         <v>171</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>14</v>
@@ -24518,16 +24515,16 @@
         <v>173</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="BL1" s="1" t="s">
         <v>174</v>
@@ -24539,7 +24536,7 @@
         <v>95</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="BP1" s="1" t="s">
         <v>27</v>
@@ -24548,7 +24545,7 @@
         <v>22</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>176</v>
@@ -24575,19 +24572,19 @@
         <v>182</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="CB1" s="1" t="s">
         <v>183</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="CF1" s="1" t="s">
         <v>184</v>
@@ -24608,16 +24605,16 @@
         <v>189</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="CP1" s="1" t="s">
         <v>191</v>
@@ -24626,10 +24623,10 @@
         <v>192</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="CT1" s="1" t="s">
         <v>93</v>
@@ -24638,22 +24635,22 @@
         <v>193</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>194</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>195</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="DB1" s="1" t="s">
         <v>196</v>
@@ -24668,7 +24665,7 @@
         <v>199</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="DG1" s="1" t="s">
         <v>200</v>
@@ -24677,10 +24674,10 @@
         <v>26</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="DK1" s="1" t="s">
         <v>201</v>
@@ -24698,19 +24695,19 @@
         <v>203</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>204</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="DT1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="DU1" s="1" t="s">
         <v>205</v>
@@ -24722,7 +24719,7 @@
         <v>91</v>
       </c>
       <c r="DX1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="DY1" s="1" t="s">
         <v>207</v>
@@ -24731,7 +24728,7 @@
         <v>208</v>
       </c>
       <c r="EA1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="EB1" s="1" t="s">
         <v>96</v>
@@ -24749,16 +24746,16 @@
         <v>212</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="EH1" s="1" t="s">
         <v>213</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="EK1" s="1" t="s">
         <v>214</v>
@@ -24767,7 +24764,7 @@
         <v>215</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="EN1" s="1" t="s">
         <v>216</v>
@@ -24779,13 +24776,13 @@
         <v>218</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="ER1" s="1" t="s">
         <v>99</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="ET1" s="1" t="s">
         <v>219</v>
@@ -24818,10 +24815,10 @@
         <v>24</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="FF1" s="1" t="s">
         <v>225</v>
@@ -24839,22 +24836,22 @@
         <v>228</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="FL1" s="1" t="s">
         <v>229</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="FN1" s="1" t="s">
         <v>230</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="FQ1" s="1" t="s">
         <v>231</v>
@@ -24863,13 +24860,13 @@
         <v>232</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="FT1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="FV1" s="1" t="s">
         <v>98</v>
@@ -28851,7 +28848,7 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -28967,7 +28964,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -29199,7 +29196,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>39</v>
@@ -29315,7 +29312,7 @@
     </row>
     <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>57</v>
@@ -29547,7 +29544,7 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -29779,7 +29776,7 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -29895,7 +29892,7 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -30011,7 +30008,7 @@
     </row>
     <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12">
         <v>44</v>
@@ -30127,7 +30124,7 @@
     </row>
     <row r="13" spans="1:38">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B13">
         <v>13</v>
@@ -30243,7 +30240,7 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>131</v>
@@ -30359,10 +30356,10 @@
     </row>
     <row r="15" spans="1:38">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -30371,37 +30368,37 @@
         <v>138</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>180.64</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -30475,7 +30472,7 @@
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>77</v>
@@ -30591,7 +30588,7 @@
     </row>
     <row r="17" spans="1:38">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <v>76</v>
@@ -30707,7 +30704,7 @@
     </row>
     <row r="18" spans="1:38">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -31171,7 +31168,7 @@
     </row>
     <row r="22" spans="1:38">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>39</v>
@@ -31287,7 +31284,7 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23">
         <v>132</v>
@@ -31403,7 +31400,7 @@
     </row>
     <row r="24" spans="1:38">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>59</v>
@@ -31519,7 +31516,7 @@
     </row>
     <row r="25" spans="1:38">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25">
         <v>27</v>

</xml_diff>